<commit_message>
bufferCell boundingRect fixed, many fixes for loading previous projects;
</commit_message>
<xml_diff>
--- a/resources/Pin expl.xlsx
+++ b/resources/Pin expl.xlsx
@@ -495,12 +495,14 @@
   <dimension ref="M11:AN31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="320" width="3.7109375" customWidth="1"/>
+    <col min="1" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="40" width="2.7109375" customWidth="1"/>
+    <col min="41" max="320" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="11" spans="13:40" x14ac:dyDescent="0.25">
@@ -663,7 +665,7 @@
       </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="5" t="str">
-        <f t="shared" ref="Q18:AN18" si="0">R15</f>
+        <f t="shared" ref="Q18" si="0">R15</f>
         <v>NC</v>
       </c>
       <c r="R18" s="9"/>
@@ -672,7 +674,7 @@
       </c>
       <c r="T18" s="6"/>
       <c r="U18" s="5" t="str">
-        <f t="shared" ref="U18:AN18" si="1">V15</f>
+        <f t="shared" ref="U18" si="1">V15</f>
         <v>D</v>
       </c>
       <c r="V18" s="9"/>
@@ -681,7 +683,7 @@
       </c>
       <c r="X18" s="6"/>
       <c r="Y18" s="5" t="str">
-        <f t="shared" ref="Y18:AN18" si="2">Z15</f>
+        <f t="shared" ref="Y18" si="2">Z15</f>
         <v>Q</v>
       </c>
       <c r="Z18" s="9"/>
@@ -690,7 +692,7 @@
       </c>
       <c r="AB18" s="6"/>
       <c r="AC18" s="5" t="str">
-        <f t="shared" ref="AC18:AN18" si="3">AD15</f>
+        <f t="shared" ref="AC18" si="3">AD15</f>
         <v>*</v>
       </c>
       <c r="AD18" s="9"/>
@@ -699,7 +701,7 @@
       </c>
       <c r="AF18" s="6"/>
       <c r="AG18" s="5" t="str">
-        <f t="shared" ref="AG18:AN18" si="4">AH15</f>
+        <f t="shared" ref="AG18" si="4">AH15</f>
         <v>SR</v>
       </c>
       <c r="AH18" s="9"/>
@@ -708,7 +710,7 @@
       </c>
       <c r="AJ18" s="6"/>
       <c r="AK18" s="5" t="str">
-        <f t="shared" ref="AK18:AN18" si="5">AL15</f>
+        <f t="shared" ref="AK18" si="5">AL15</f>
         <v>*</v>
       </c>
       <c r="AL18" s="9"/>

</xml_diff>